<commit_message>
continue valuation kalika toilet and kurthali truss and sanagaun dhal byabasthapan quantity for vat
</commit_message>
<xml_diff>
--- a/ofc/estimates/sana gaun dhal byabasthapan/V_with hume pipe-sanagaun dhal byabasthapan.xlsx
+++ b/ofc/estimates/sana gaun dhal byabasthapan/V_with hume pipe-sanagaun dhal byabasthapan.xlsx
@@ -2,32 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\estimates\sana gaun dhal byabasthapan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\sana gaun dhal byabasthapan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate (3)" sheetId="19" r:id="rId1"/>
     <sheet name="WCR" sheetId="6" r:id="rId2"/>
     <sheet name="Valuated" sheetId="21" r:id="rId3"/>
-    <sheet name="V" sheetId="20" state="hidden" r:id="rId4"/>
+    <sheet name="M" sheetId="22" r:id="rId4"/>
+    <sheet name="V" sheetId="20" state="hidden" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="0">#REF!</definedName>
     <definedName name="description_124" localSheetId="3">#REF!</definedName>
+    <definedName name="description_124" localSheetId="4">#REF!</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
@@ -43,15 +45,16 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Estimate (3)'!$A$1:$K$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">V!$A$1:$K$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">M!$A$1:$K$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">V!$A$1:$K$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Valuated!$A$1:$K$49</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Estimate (3)'!$1:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">V!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">M!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Valuated!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="76">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -264,15 +267,48 @@
   </si>
   <si>
     <t>-For drain clearance</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>VAT 13%</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>formwork</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>hume pipe</t>
+  </si>
+  <si>
+    <t>jcb</t>
+  </si>
+  <si>
+    <t>Detail Quantity Measurement Sheet</t>
+  </si>
+  <si>
+    <t>rm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -457,9 +493,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -467,7 +503,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,14 +523,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -503,7 +539,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -528,7 +564,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,7 +594,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -567,7 +603,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,7 +618,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -598,15 +634,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,22 +684,19 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -660,25 +717,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1297,137 +1339,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
       <c r="O6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1507,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -1488,7 +1530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
         <v>50</v>
@@ -1524,7 +1566,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>64</v>
@@ -1557,7 +1599,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>42</v>
@@ -1589,7 +1631,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37" t="s">
         <v>40</v>
@@ -1614,7 +1656,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="37"/>
       <c r="C14" s="19"/>
@@ -1634,7 +1676,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -1651,7 +1693,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>61</v>
@@ -1676,11 +1718,11 @@
       <c r="H16" s="22"/>
       <c r="I16" s="23"/>
       <c r="J16" s="41"/>
-      <c r="K16" s="70" t="s">
+      <c r="K16" s="78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37" t="s">
         <v>42</v>
@@ -1703,9 +1745,9 @@
         <f>G17*I17</f>
         <v>14536</v>
       </c>
-      <c r="K17" s="71"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="37"/>
       <c r="C18" s="19"/>
@@ -1720,7 +1762,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>3</v>
       </c>
@@ -1744,7 +1786,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37" t="s">
         <v>43</v>
@@ -1779,7 +1821,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -1804,7 +1846,7 @@
       </c>
       <c r="K21" s="36"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
       <c r="B22" s="37" t="s">
         <v>40</v>
@@ -1822,7 +1864,7 @@
       </c>
       <c r="K22" s="36"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="42"/>
@@ -1835,7 +1877,7 @@
       <c r="J23" s="45"/>
       <c r="K23" s="36"/>
     </row>
-    <row r="24" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>4</v>
       </c>
@@ -1859,7 +1901,7 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>50</v>
@@ -1894,7 +1936,7 @@
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37"/>
       <c r="C26" s="36">
@@ -1926,7 +1968,7 @@
       <c r="R26" s="25"/>
       <c r="S26" s="25"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="37" t="s">
         <v>42</v>
@@ -1951,7 +1993,7 @@
       </c>
       <c r="K27" s="36"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="37" t="s">
         <v>40</v>
@@ -1969,7 +2011,7 @@
       </c>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="37"/>
       <c r="C29" s="42"/>
@@ -1982,7 +2024,7 @@
       <c r="J29" s="45"/>
       <c r="K29" s="36"/>
     </row>
-    <row r="30" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A30" s="63">
         <v>5</v>
       </c>
@@ -1999,7 +2041,7 @@
       <c r="J30" s="45"/>
       <c r="K30" s="29"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37" t="s">
         <v>50</v>
@@ -2033,7 +2075,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
         <v>42</v>
@@ -2058,7 +2100,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>40</v>
@@ -2076,7 +2118,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37"/>
       <c r="C34" s="42"/>
@@ -2089,7 +2131,7 @@
       <c r="J34" s="44"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A35" s="63">
         <v>6</v>
       </c>
@@ -2106,7 +2148,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="29"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="37" t="s">
         <v>59</v>
@@ -2136,7 +2178,7 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="37" t="s">
         <v>42</v>
@@ -2150,7 +2192,7 @@
         <v>10</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I37" s="33">
         <v>5144.96</v>
@@ -2161,7 +2203,7 @@
       </c>
       <c r="K37" s="36"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="37" t="s">
         <v>40</v>
@@ -2179,7 +2221,7 @@
       </c>
       <c r="K38" s="36"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="37"/>
       <c r="C39" s="42"/>
@@ -2192,7 +2234,7 @@
       <c r="J39" s="44"/>
       <c r="K39" s="36"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <v>7</v>
       </c>
@@ -2228,7 +2270,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="24"/>
       <c r="C41" s="19"/>
@@ -2251,7 +2293,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="46" t="s">
         <v>17</v>
@@ -2269,7 +2311,7 @@
       </c>
       <c r="K42" s="36"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="58"/>
       <c r="B43" s="61"/>
       <c r="C43" s="62"/>
@@ -2282,16 +2324,16 @@
       <c r="J43" s="60"/>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50"/>
       <c r="B44" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="66">
+      <c r="C44" s="74">
         <f>J42</f>
         <v>447610.1230384605</v>
       </c>
-      <c r="D44" s="66"/>
+      <c r="D44" s="74"/>
       <c r="E44" s="39">
         <v>100</v>
       </c>
@@ -2302,15 +2344,15 @@
       <c r="J44" s="54"/>
       <c r="K44" s="55"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="56"/>
       <c r="B45" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="69">
+      <c r="C45" s="77">
         <v>400000</v>
       </c>
-      <c r="D45" s="69"/>
+      <c r="D45" s="77"/>
       <c r="E45" s="39"/>
       <c r="F45" s="49"/>
       <c r="G45" s="48"/>
@@ -2319,16 +2361,16 @@
       <c r="J45" s="48"/>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="56"/>
       <c r="B46" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="69">
+      <c r="C46" s="77">
         <f>C45-C48-C49</f>
         <v>380000</v>
       </c>
-      <c r="D46" s="69"/>
+      <c r="D46" s="77"/>
       <c r="E46" s="39">
         <f>C46/C44*100</f>
         <v>84.895309654859801</v>
@@ -2340,16 +2382,16 @@
       <c r="J46" s="48"/>
       <c r="K46" s="49"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="56"/>
       <c r="B47" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="66">
+      <c r="C47" s="74">
         <f>C44-C46</f>
         <v>67610.123038460501</v>
       </c>
-      <c r="D47" s="66"/>
+      <c r="D47" s="74"/>
       <c r="E47" s="39">
         <f>100-E46</f>
         <v>15.104690345140199</v>
@@ -2361,16 +2403,16 @@
       <c r="J47" s="48"/>
       <c r="K47" s="49"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="56"/>
       <c r="B48" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="66">
+      <c r="C48" s="74">
         <f>C45*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D48" s="66"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="39">
         <v>3</v>
       </c>
@@ -2381,16 +2423,16 @@
       <c r="J48" s="48"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="56"/>
       <c r="B49" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="66">
+      <c r="C49" s="74">
         <f>C45*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D49" s="66"/>
+      <c r="D49" s="74"/>
       <c r="E49" s="39">
         <v>2</v>
       </c>
@@ -2401,7 +2443,7 @@
       <c r="J49" s="48"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="57"/>
       <c r="B50" s="57"/>
       <c r="C50" s="57"/>
@@ -2414,71 +2456,64 @@
       <c r="J50" s="57"/>
       <c r="K50" s="57"/>
     </row>
-    <row r="51" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="A7:F7"/>
@@ -2488,6 +2523,13 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="K16:K17"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2501,110 +2543,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-    </row>
-    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="87" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+    </row>
+    <row r="2" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="88" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="84">
+      <c r="C6" s="80">
         <f>F32</f>
         <v>447610.1230384605</v>
       </c>
-      <c r="D6" s="85"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2612,90 +2654,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="84">
+      <c r="J6" s="80">
         <f>I32</f>
         <v>448359.42496248247</v>
       </c>
-      <c r="K6" s="85"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="81"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="I7" s="81" t="s">
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="I7" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="str">
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="68" t="str">
         <f>'Estimate (3)'!A6:F6</f>
         <v xml:space="preserve">Project:- सानागाउँ ढल व्यबस्थापन </v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="I8" s="82" t="s">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="I8" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="str">
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="68" t="str">
         <f>'Estimate (3)'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="I9" s="82" t="s">
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="I9" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83" t="s">
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="78" t="s">
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="85"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2714,10 +2756,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="79"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="85"/>
+      <c r="K12" s="86"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <f>'Estimate (3)'!A9</f>
         <v>1</v>
@@ -2764,7 +2806,7 @@
         <v>5015.1365234374998</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="65" t="str">
         <f>'Estimate (3)'!B13</f>
@@ -2793,7 +2835,7 @@
         <v>540.36421223958337</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="32"/>
       <c r="C15" s="12"/>
@@ -2806,7 +2848,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="27">
         <f>'Estimate (3)'!A15</f>
         <v>2</v>
@@ -2853,7 +2895,7 @@
         <v>18170</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
       <c r="B17" s="32"/>
       <c r="C17" s="12"/>
@@ -2866,7 +2908,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A18" s="27">
         <f>'Estimate (3)'!A19</f>
         <v>3</v>
@@ -2913,7 +2955,7 @@
         <v>15288.252890624999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="65" t="str">
         <f>'Estimate (3)'!B22</f>
@@ -2942,7 +2984,7 @@
         <v>1346.5492218750001</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="32"/>
       <c r="C20" s="12"/>
@@ -2955,7 +2997,7 @@
       <c r="J20" s="28"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A21" s="27">
         <f>'Estimate (3)'!A24</f>
         <v>4</v>
@@ -3002,7 +3044,7 @@
         <v>22141.361328125</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="65" t="str">
         <f>'Estimate (3)'!B28</f>
@@ -3031,7 +3073,7 @@
         <v>2184.1254567708338</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="32"/>
       <c r="C23" s="12"/>
@@ -3044,7 +3086,7 @@
       <c r="J23" s="28"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A24" s="27">
         <f>'Estimate (3)'!A30</f>
         <v>5</v>
@@ -3091,7 +3133,7 @@
         <v>393858.99201302679</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="27"/>
       <c r="B25" s="65" t="str">
         <f>'Estimate (3)'!B33</f>
@@ -3120,7 +3162,7 @@
         <v>28573.474151975883</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="27"/>
       <c r="B26" s="32"/>
       <c r="C26" s="12"/>
@@ -3133,7 +3175,7 @@
       <c r="J26" s="28"/>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <f>'Estimate (3)'!A35</f>
         <v>6</v>
@@ -3144,7 +3186,7 @@
       </c>
       <c r="C27" s="12" t="str">
         <f>'Estimate (3)'!H37</f>
-        <v>m3</v>
+        <v>rm</v>
       </c>
       <c r="D27" s="12">
         <f>'Estimate (3)'!G37</f>
@@ -3176,7 +3218,7 @@
       </c>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="27"/>
       <c r="B28" s="65" t="str">
         <f>'Estimate (3)'!B38</f>
@@ -3201,7 +3243,7 @@
       </c>
       <c r="K28" s="14"/>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
       <c r="B29" s="32"/>
       <c r="C29" s="12"/>
@@ -3214,7 +3256,7 @@
       <c r="J29" s="28"/>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <f>'Estimate (3)'!A40</f>
         <v>7</v>
@@ -3261,7 +3303,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="12"/>
@@ -3274,7 +3316,7 @@
       <c r="J31" s="28"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
         <v>16</v>
@@ -3300,13 +3342,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3320,6 +3355,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3335,139 +3377,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S106"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="O6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3501,11 +3544,8 @@
       <c r="K8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -3521,14 +3561,8 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
-      <c r="N9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
         <v>50</v>
@@ -3554,15 +3588,8 @@
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="21"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>64</v>
@@ -3587,15 +3614,8 @@
       <c r="I11" s="40"/>
       <c r="J11" s="40"/>
       <c r="K11" s="21"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>42</v>
@@ -3619,15 +3639,8 @@
         <v>4544.296875</v>
       </c>
       <c r="K12" s="21"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37" t="s">
         <v>40</v>
@@ -3644,15 +3657,8 @@
         <v>489.6328125</v>
       </c>
       <c r="K13" s="21"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-    </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="37"/>
       <c r="C14" s="19"/>
@@ -3664,15 +3670,8 @@
       <c r="I14" s="23"/>
       <c r="J14" s="41"/>
       <c r="K14" s="21"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3689,7 +3688,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>61</v>
@@ -3714,11 +3713,11 @@
       <c r="H16" s="22"/>
       <c r="I16" s="23"/>
       <c r="J16" s="41"/>
-      <c r="K16" s="70" t="s">
+      <c r="K16" s="78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37" t="s">
         <v>42</v>
@@ -3741,9 +3740,9 @@
         <f>G17*I17</f>
         <v>14536</v>
       </c>
-      <c r="K17" s="71"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="37"/>
       <c r="C18" s="19"/>
@@ -3755,10 +3754,8 @@
       <c r="I18" s="23"/>
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-    </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>3</v>
       </c>
@@ -3774,15 +3771,21 @@
       <c r="I19" s="23"/>
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" s="91"/>
+      <c r="R19" s="91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37" t="s">
         <v>43</v>
@@ -3809,15 +3812,24 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="21"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="O20" s="92">
+        <f>19284/360*G12</f>
+        <v>3766.4062500000005</v>
+      </c>
+      <c r="P20" s="92">
+        <f>O20*0.13</f>
+        <v>489.63281250000006</v>
+      </c>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="92">
+        <f t="shared" ref="R20" si="0">SUM(O20:P20)</f>
+        <v>4256.0390625000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -3841,8 +3853,24 @@
         <v>13044.363067662298</v>
       </c>
       <c r="K21" s="36"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N21" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="O21" s="92">
+        <f>15452.6/5*G21+14808.78/5*G32</f>
+        <v>104407.40270230114</v>
+      </c>
+      <c r="P21" s="92">
+        <f>O21*0.13</f>
+        <v>13572.962351299149</v>
+      </c>
+      <c r="Q21" s="92"/>
+      <c r="R21" s="92">
+        <f t="shared" ref="R21:R26" si="1">SUM(O21:P21)</f>
+        <v>117980.3650536003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
       <c r="B22" s="37" t="s">
         <v>40</v>
@@ -3859,8 +3887,24 @@
         <v>1148.9132907650107</v>
       </c>
       <c r="K22" s="36"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="O22" s="92">
+        <f>49275.03/15*G27+5368.95/5*G32+835.17/12.5*G37</f>
+        <v>41122.730792075585</v>
+      </c>
+      <c r="P22" s="92">
+        <f>O22*0.13</f>
+        <v>5345.9550029698266</v>
+      </c>
+      <c r="Q22" s="92"/>
+      <c r="R22" s="92">
+        <f t="shared" si="1"/>
+        <v>46468.685795045414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="42"/>
@@ -3872,8 +3916,24 @@
       <c r="I23" s="43"/>
       <c r="J23" s="45"/>
       <c r="K23" s="36"/>
-    </row>
-    <row r="24" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="N23" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="92">
+        <f>21432.6/15*G27+6604.42/5*G32+279.42/12.5*G37</f>
+        <v>45370.893870237727</v>
+      </c>
+      <c r="P23" s="92">
+        <f t="shared" ref="P23:P27" si="2">O23*0.13</f>
+        <v>5898.2162031309044</v>
+      </c>
+      <c r="Q23" s="92"/>
+      <c r="R23" s="92">
+        <f t="shared" si="1"/>
+        <v>51269.110073368633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="69" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>4</v>
       </c>
@@ -3889,15 +3949,24 @@
       <c r="I24" s="23"/>
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N24" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="O24" s="92">
+        <f>(25719.12+13573.98+4286.52)/15*G27</f>
+        <v>5134.618303093569</v>
+      </c>
+      <c r="P24" s="92">
+        <f t="shared" si="2"/>
+        <v>667.50037940216396</v>
+      </c>
+      <c r="Q24" s="92"/>
+      <c r="R24" s="92">
+        <f t="shared" si="1"/>
+        <v>5802.1186824957331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>50</v>
@@ -3924,18 +3993,24 @@
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
       <c r="K25" s="21"/>
-      <c r="M25" s="39">
-        <f>4.17/3.281</f>
-        <v>1.2709539774459007</v>
-      </c>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N25" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="O25" s="92">
+        <f>6135.3/15*G27</f>
+        <v>722.8705453367877</v>
+      </c>
+      <c r="P25" s="92">
+        <f t="shared" si="2"/>
+        <v>93.97317089378241</v>
+      </c>
+      <c r="Q25" s="92"/>
+      <c r="R25" s="92">
+        <f t="shared" si="1"/>
+        <v>816.84371623057007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37"/>
       <c r="C26" s="36">
@@ -3959,15 +4034,24 @@
       <c r="I26" s="40"/>
       <c r="J26" s="40"/>
       <c r="K26" s="21"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N26" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="92">
+        <f>310/5*G32+620/15*G27</f>
+        <v>2073.6583587320938</v>
+      </c>
+      <c r="P26" s="92">
+        <f t="shared" si="2"/>
+        <v>269.57558663517221</v>
+      </c>
+      <c r="Q26" s="92"/>
+      <c r="R26" s="92">
+        <f t="shared" si="1"/>
+        <v>2343.2339453672662</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="37" t="s">
         <v>42</v>
@@ -3991,8 +4075,24 @@
         <v>18794.598832291987</v>
       </c>
       <c r="K27" s="36"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N27" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="O27" s="92">
+        <f>56250/12.5*G37</f>
+        <v>45000</v>
+      </c>
+      <c r="P27" s="92">
+        <f t="shared" si="2"/>
+        <v>5850</v>
+      </c>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92">
+        <f>SUM(O27:P27)</f>
+        <v>50850</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="37" t="s">
         <v>40</v>
@@ -4010,7 +4110,7 @@
       </c>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="37"/>
       <c r="C29" s="42"/>
@@ -4023,7 +4123,7 @@
       <c r="J29" s="45"/>
       <c r="K29" s="36"/>
     </row>
-    <row r="30" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A30" s="63">
         <v>5</v>
       </c>
@@ -4040,7 +4140,7 @@
       <c r="J30" s="45"/>
       <c r="K30" s="29"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37" t="s">
         <v>50</v>
@@ -4066,15 +4166,8 @@
       <c r="I31" s="40"/>
       <c r="J31" s="40"/>
       <c r="K31" s="21"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="89"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
         <v>42</v>
@@ -4099,7 +4192,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>40</v>
@@ -4117,7 +4210,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37"/>
       <c r="C34" s="42"/>
@@ -4130,7 +4223,7 @@
       <c r="J34" s="44"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A35" s="63">
         <v>6</v>
       </c>
@@ -4147,7 +4240,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="29"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="37" t="s">
         <v>59</v>
@@ -4169,15 +4262,8 @@
       <c r="I36" s="40"/>
       <c r="J36" s="40"/>
       <c r="K36" s="21"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-    </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="37" t="s">
         <v>42</v>
@@ -4191,7 +4277,7 @@
         <v>10</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I37" s="33">
         <v>5144.96</v>
@@ -4202,7 +4288,7 @@
       </c>
       <c r="K37" s="36"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="37" t="s">
         <v>40</v>
@@ -4220,7 +4306,7 @@
       </c>
       <c r="K38" s="36"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="37"/>
       <c r="C39" s="42"/>
@@ -4233,7 +4319,7 @@
       <c r="J39" s="44"/>
       <c r="K39" s="36"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <v>7</v>
       </c>
@@ -4247,7 +4333,7 @@
       <c r="E40" s="21"/>
       <c r="F40" s="21"/>
       <c r="G40" s="34">
-        <f t="shared" ref="G40" si="0">PRODUCT(C40:F40)</f>
+        <f t="shared" ref="G40" si="3">PRODUCT(C40:F40)</f>
         <v>1</v>
       </c>
       <c r="H40" s="22" t="s">
@@ -4261,15 +4347,8 @@
         <v>500</v>
       </c>
       <c r="K40" s="21"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="24"/>
       <c r="C41" s="19"/>
@@ -4281,18 +4360,8 @@
       <c r="I41" s="23"/>
       <c r="J41" s="41"/>
       <c r="K41" s="21"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="1">
-        <f>2.4*3.281</f>
-        <v>7.8743999999999996</v>
-      </c>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="46" t="s">
         <v>17</v>
@@ -4310,7 +4379,7 @@
       </c>
       <c r="K42" s="36"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="58"/>
       <c r="B43" s="61"/>
       <c r="C43" s="62"/>
@@ -4323,16 +4392,16 @@
       <c r="J43" s="60"/>
       <c r="K43" s="57"/>
     </row>
-    <row r="44" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50"/>
       <c r="B44" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="66">
+      <c r="C44" s="74">
         <f>J42</f>
         <v>448359.42496248247</v>
       </c>
-      <c r="D44" s="66"/>
+      <c r="D44" s="74"/>
       <c r="E44" s="39">
         <v>100</v>
       </c>
@@ -4343,15 +4412,15 @@
       <c r="J44" s="54"/>
       <c r="K44" s="55"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="56"/>
       <c r="B45" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="69">
+      <c r="C45" s="77">
         <v>400000</v>
       </c>
-      <c r="D45" s="69"/>
+      <c r="D45" s="77"/>
       <c r="E45" s="39"/>
       <c r="F45" s="49"/>
       <c r="G45" s="48"/>
@@ -4360,16 +4429,16 @@
       <c r="J45" s="48"/>
       <c r="K45" s="49"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="56"/>
       <c r="B46" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="69">
+      <c r="C46" s="77">
         <f>C45-C48-C49</f>
         <v>380000</v>
       </c>
-      <c r="D46" s="69"/>
+      <c r="D46" s="77"/>
       <c r="E46" s="39">
         <f>C46/C44*100</f>
         <v>84.753431921676992</v>
@@ -4381,16 +4450,16 @@
       <c r="J46" s="48"/>
       <c r="K46" s="49"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="56"/>
       <c r="B47" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="66">
+      <c r="C47" s="74">
         <f>C44-C46</f>
         <v>68359.424962482473</v>
       </c>
-      <c r="D47" s="66"/>
+      <c r="D47" s="74"/>
       <c r="E47" s="39">
         <f>100-E46</f>
         <v>15.246568078323008</v>
@@ -4402,16 +4471,16 @@
       <c r="J47" s="48"/>
       <c r="K47" s="49"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="56"/>
       <c r="B48" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="66">
+      <c r="C48" s="74">
         <f>C45*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D48" s="66"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="39">
         <v>3</v>
       </c>
@@ -4422,16 +4491,16 @@
       <c r="J48" s="48"/>
       <c r="K48" s="49"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="56"/>
       <c r="B49" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="66">
+      <c r="C49" s="74">
         <f>C45*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D49" s="66"/>
+      <c r="D49" s="74"/>
       <c r="E49" s="39">
         <v>2</v>
       </c>
@@ -4442,7 +4511,7 @@
       <c r="J49" s="48"/>
       <c r="K49" s="49"/>
     </row>
-    <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="57"/>
       <c r="B50" s="57"/>
       <c r="C50" s="57"/>
@@ -4455,64 +4524,71 @@
       <c r="J50" s="57"/>
       <c r="K50" s="57"/>
     </row>
-    <row r="51" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
@@ -4522,13 +4598,6 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -4540,136 +4609,140 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S100"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="73" t="s">
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="68" t="s">
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -4704,7 +4777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -4721,7 +4794,1233 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="38">
+        <f>D31</f>
+        <v>15</v>
+      </c>
+      <c r="E10" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="F10" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="39">
+        <f>PRODUCT(C10:F10)</f>
+        <v>14.0625</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="36">
+        <v>1</v>
+      </c>
+      <c r="D11" s="38">
+        <v>50</v>
+      </c>
+      <c r="E11" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="39">
+        <f>PRODUCT(C11:F11)</f>
+        <v>56.25</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>70.3125</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
+      <c r="J12" s="41">
+        <f>G12*I12</f>
+        <v>4544.296875</v>
+      </c>
+      <c r="K12" s="21"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="41">
+        <f>0.13*G12*19284/360</f>
+        <v>489.6328125</v>
+      </c>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
+      <c r="D16" s="20">
+        <v>30</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.38</v>
+      </c>
+      <c r="F16" s="38">
+        <f>ROUNDUP(D16/E16,0)</f>
+        <v>79</v>
+      </c>
+      <c r="G16" s="39">
+        <f>F16*C16</f>
+        <v>158</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="78" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="23">
+        <f>SUM(G16:G16)</f>
+        <v>158</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="23">
+        <v>92</v>
+      </c>
+      <c r="J17" s="41">
+        <f>G17*I17</f>
+        <v>14536</v>
+      </c>
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:18" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>3</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="21"/>
+      <c r="N19" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" s="91"/>
+      <c r="R19" s="91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="36">
+        <v>1</v>
+      </c>
+      <c r="D20" s="38">
+        <f>D25</f>
+        <v>15</v>
+      </c>
+      <c r="E20" s="38">
+        <f>E25</f>
+        <v>1.2709539774459007</v>
+      </c>
+      <c r="F20" s="38">
+        <v>0.15</v>
+      </c>
+      <c r="G20" s="39">
+        <f>PRODUCT(C20:F20)</f>
+        <v>2.8596464492532765</v>
+      </c>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="21"/>
+      <c r="N20" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="O20" s="92">
+        <f>19284/360*G12</f>
+        <v>3766.4062500000005</v>
+      </c>
+      <c r="P20" s="92">
+        <f>O20*0.13</f>
+        <v>489.63281250000006</v>
+      </c>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="92">
+        <f t="shared" ref="R20:R26" si="0">SUM(O20:P20)</f>
+        <v>4256.0390625000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="33">
+        <f>SUM(G20:G20)</f>
+        <v>2.8596464492532765</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="33">
+        <v>4561.53</v>
+      </c>
+      <c r="J21" s="44">
+        <f>G21*I21</f>
+        <v>13044.363067662298</v>
+      </c>
+      <c r="K21" s="36"/>
+      <c r="N21" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="O21" s="92">
+        <f>15452.6/5*G21+14808.78/5*G32</f>
+        <v>104407.40270230114</v>
+      </c>
+      <c r="P21" s="92">
+        <f>O21*0.13</f>
+        <v>13572.962351299149</v>
+      </c>
+      <c r="Q21" s="92"/>
+      <c r="R21" s="92">
+        <f t="shared" si="0"/>
+        <v>117980.3650536003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40"/>
+      <c r="B22" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="45">
+        <f>0.13*G21*(15452.6/5)</f>
+        <v>1148.9132907650107</v>
+      </c>
+      <c r="K22" s="36"/>
+      <c r="N22" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="O22" s="92">
+        <f>49275.03/15*G27+5368.95/5*G32+835.17/12.5*G37</f>
+        <v>41122.730792075585</v>
+      </c>
+      <c r="P22" s="92">
+        <f>O22*0.13</f>
+        <v>5345.9550029698266</v>
+      </c>
+      <c r="Q22" s="92"/>
+      <c r="R22" s="92">
+        <f t="shared" si="0"/>
+        <v>46468.685795045414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="36"/>
+      <c r="N23" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="92">
+        <f>21432.6/15*G27+6604.42/5*G32+279.42/12.5*G37</f>
+        <v>45370.893870237727</v>
+      </c>
+      <c r="P23" s="92">
+        <f t="shared" ref="P23:P27" si="1">O23*0.13</f>
+        <v>5898.2162031309044</v>
+      </c>
+      <c r="Q23" s="92"/>
+      <c r="R23" s="92">
+        <f t="shared" si="0"/>
+        <v>51269.110073368633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="69" x14ac:dyDescent="0.3">
+      <c r="A24" s="18">
+        <v>4</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="21"/>
+      <c r="N24" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="O24" s="92">
+        <f>(25719.12+13573.98+4286.52)/15*G27</f>
+        <v>5134.618303093569</v>
+      </c>
+      <c r="P24" s="92">
+        <f t="shared" si="1"/>
+        <v>667.50037940216396</v>
+      </c>
+      <c r="Q24" s="92"/>
+      <c r="R24" s="92">
+        <f t="shared" si="0"/>
+        <v>5802.1186824957331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="36">
+        <v>1</v>
+      </c>
+      <c r="D25" s="38">
+        <f>D31</f>
+        <v>15</v>
+      </c>
+      <c r="E25" s="38">
+        <f>4.17/3.281</f>
+        <v>1.2709539774459007</v>
+      </c>
+      <c r="F25" s="38">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G25" s="39">
+        <f>PRODUCT(C25:F25)</f>
+        <v>1.4298232246266382</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="21"/>
+      <c r="N25" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="O25" s="92">
+        <f>6135.3/15*G27</f>
+        <v>722.8705453367877</v>
+      </c>
+      <c r="P25" s="92">
+        <f t="shared" si="1"/>
+        <v>93.97317089378241</v>
+      </c>
+      <c r="Q25" s="92"/>
+      <c r="R25" s="92">
+        <f t="shared" si="0"/>
+        <v>816.84371623057007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36">
+        <v>1</v>
+      </c>
+      <c r="D26" s="38">
+        <f>D25</f>
+        <v>15</v>
+      </c>
+      <c r="E26" s="38">
+        <v>0.45</v>
+      </c>
+      <c r="F26" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="G26" s="39">
+        <f>PRODUCT(C26:F26)</f>
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="21"/>
+      <c r="N26" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="92">
+        <f>310/5*G32+620/15*G27</f>
+        <v>2073.6583587320938</v>
+      </c>
+      <c r="P26" s="92">
+        <f t="shared" si="1"/>
+        <v>269.57558663517221</v>
+      </c>
+      <c r="Q26" s="92"/>
+      <c r="R26" s="92">
+        <f t="shared" si="0"/>
+        <v>2343.2339453672662</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="40"/>
+      <c r="B27" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="33">
+        <f>SUM(G25:G26)</f>
+        <v>1.7673232246266384</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="33">
+        <v>10634.5</v>
+      </c>
+      <c r="J27" s="44">
+        <f>G27*I27</f>
+        <v>18794.598832291987</v>
+      </c>
+      <c r="K27" s="36"/>
+      <c r="N27" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="O27" s="92">
+        <f>56250/12.5*G37</f>
+        <v>45000</v>
+      </c>
+      <c r="P27" s="92">
+        <f t="shared" si="1"/>
+        <v>5850</v>
+      </c>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92">
+        <f>SUM(O27:P27)</f>
+        <v>50850</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="40"/>
+      <c r="B28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="45">
+        <f>0.13*G27*((114907.3+6135.3)/15)</f>
+        <v>1853.9854506263337</v>
+      </c>
+      <c r="K28" s="36"/>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="40"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="1:18" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="63">
+        <v>5</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="64"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="36">
+        <v>1</v>
+      </c>
+      <c r="D31" s="38">
+        <v>15</v>
+      </c>
+      <c r="E31" s="38">
+        <f>((4.17/3.281+0.45)/2)</f>
+        <v>0.86047698872295031</v>
+      </c>
+      <c r="F31" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="G31" s="39">
+        <f>PRODUCT(C31:F31)</f>
+        <v>32.267887077110636</v>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="40"/>
+      <c r="B32" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="33">
+        <f>SUM(G31:G31)</f>
+        <v>32.267887077110636</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="33">
+        <v>9709.43</v>
+      </c>
+      <c r="J32" s="44">
+        <f>G32*I32</f>
+        <v>313302.79082311032</v>
+      </c>
+      <c r="K32" s="36"/>
+    </row>
+    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="40"/>
+      <c r="B33" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="45">
+        <f>0.13*G32*((27092.1)/5)</f>
+        <v>22729.325410526515</v>
+      </c>
+      <c r="K33" s="36"/>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="40"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="36"/>
+    </row>
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="63">
+        <v>6</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="64"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="29"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="36">
+        <v>4</v>
+      </c>
+      <c r="D36" s="38">
+        <f>2.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39">
+        <f>PRODUCT(C36:F36)</f>
+        <v>10</v>
+      </c>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="40"/>
+      <c r="B37" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="33">
+        <f>SUM(G36:G36)</f>
+        <v>10</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="33">
+        <v>5144.96</v>
+      </c>
+      <c r="J37" s="44">
+        <f>G37*I37</f>
+        <v>51449.599999999999</v>
+      </c>
+      <c r="K37" s="36"/>
+    </row>
+    <row r="38" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="40"/>
+      <c r="B38" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="42"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="45">
+        <f>0.13*G37*((57364.6)/12.5)</f>
+        <v>5965.9183999999996</v>
+      </c>
+      <c r="K38" s="36"/>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="40"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="36"/>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>7</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="19">
+        <v>1</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="34">
+        <f t="shared" ref="G40" si="2">PRODUCT(C40:F40)</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="23">
+        <v>500</v>
+      </c>
+      <c r="J40" s="34">
+        <f>G40*I40</f>
+        <v>500</v>
+      </c>
+      <c r="K40" s="21"/>
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="21"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="40"/>
+      <c r="B42" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41">
+        <f>SUM(J10:J40)</f>
+        <v>448359.42496248247</v>
+      </c>
+      <c r="K42" s="36"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="58"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="57"/>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="50"/>
+      <c r="B44" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="74">
+        <f>J42</f>
+        <v>448359.42496248247</v>
+      </c>
+      <c r="D44" s="74"/>
+      <c r="E44" s="39">
+        <v>100</v>
+      </c>
+      <c r="F44" s="51"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="55"/>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="56"/>
+      <c r="B45" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="77">
+        <v>400000</v>
+      </c>
+      <c r="D45" s="77"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="49"/>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="56"/>
+      <c r="B46" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="77">
+        <f>C45-C48-C49</f>
+        <v>380000</v>
+      </c>
+      <c r="D46" s="77"/>
+      <c r="E46" s="39">
+        <f>C46/C44*100</f>
+        <v>84.753431921676992</v>
+      </c>
+      <c r="F46" s="49"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="49"/>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="56"/>
+      <c r="B47" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="74">
+        <f>C44-C46</f>
+        <v>68359.424962482473</v>
+      </c>
+      <c r="D47" s="74"/>
+      <c r="E47" s="39">
+        <f>100-E46</f>
+        <v>15.246568078323008</v>
+      </c>
+      <c r="F47" s="49"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="49"/>
+    </row>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="56"/>
+      <c r="B48" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="74">
+        <f>C45*0.03</f>
+        <v>12000</v>
+      </c>
+      <c r="D48" s="74"/>
+      <c r="E48" s="39">
+        <v>3</v>
+      </c>
+      <c r="F48" s="49"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="49"/>
+    </row>
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="56"/>
+      <c r="B49" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="74">
+        <f>C45*0.02</f>
+        <v>8000</v>
+      </c>
+      <c r="D49" s="74"/>
+      <c r="E49" s="39">
+        <v>2</v>
+      </c>
+      <c r="F49" s="49"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="49"/>
+    </row>
+    <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="57"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+    </row>
+    <row r="51" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="138" x14ac:dyDescent="0.3">
+      <c r="A9" s="63">
+        <v>1</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="s">
         <v>50</v>
@@ -4751,7 +6050,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -4778,7 +6077,7 @@
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -4798,7 +6097,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -4813,7 +6112,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
     </row>
-    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -4830,7 +6129,7 @@
       <c r="J14" s="41"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>61</v>
@@ -4855,11 +6154,11 @@
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
       <c r="J15" s="41"/>
-      <c r="K15" s="70" t="s">
+      <c r="K15" s="78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>42</v>
@@ -4882,9 +6181,9 @@
         <f>G16*I16</f>
         <v>14536</v>
       </c>
-      <c r="K16" s="71"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="79"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="19"/>
@@ -4899,7 +6198,7 @@
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>4</v>
       </c>
@@ -4918,7 +6217,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="37" t="s">
         <v>50</v>
@@ -4948,7 +6247,7 @@
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37"/>
       <c r="C20" s="36">
@@ -4975,7 +6274,7 @@
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -5000,7 +6299,7 @@
       </c>
       <c r="K21" s="36"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
       <c r="B22" s="37" t="s">
         <v>40</v>
@@ -5018,7 +6317,7 @@
       </c>
       <c r="K22" s="36"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="42"/>
@@ -5031,7 +6330,7 @@
       <c r="J23" s="45"/>
       <c r="K23" s="36"/>
     </row>
-    <row r="24" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A24" s="63">
         <v>5</v>
       </c>
@@ -5048,7 +6347,7 @@
       <c r="J24" s="45"/>
       <c r="K24" s="29"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>50</v>
@@ -5080,7 +6379,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="37" t="s">
         <v>42</v>
@@ -5105,7 +6404,7 @@
       </c>
       <c r="K26" s="36"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="37" t="s">
         <v>40</v>
@@ -5139,7 +6438,7 @@
         <v>2.5397744590064004</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="37"/>
       <c r="C28" s="42"/>
@@ -5152,7 +6451,7 @@
       <c r="J28" s="44"/>
       <c r="K28" s="36"/>
     </row>
-    <row r="29" spans="1:19" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A29" s="63">
         <v>6</v>
       </c>
@@ -5169,7 +6468,7 @@
       <c r="J29" s="45"/>
       <c r="K29" s="29"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="37" t="s">
         <v>59</v>
@@ -5199,7 +6498,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="37" t="s">
         <v>42</v>
@@ -5224,7 +6523,7 @@
       </c>
       <c r="K31" s="36"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
         <v>40</v>
@@ -5242,7 +6541,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37"/>
       <c r="C33" s="42"/>
@@ -5255,7 +6554,7 @@
       <c r="J33" s="44"/>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
         <v>6</v>
       </c>
@@ -5286,7 +6585,7 @@
       <c r="M34" s="25"/>
       <c r="N34" s="25"/>
     </row>
-    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18"/>
       <c r="B35" s="24"/>
       <c r="C35" s="19"/>
@@ -5301,7 +6600,7 @@
       <c r="M35" s="25"/>
       <c r="N35" s="25"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
       <c r="B36" s="46" t="s">
         <v>17</v>
@@ -5319,7 +6618,7 @@
       </c>
       <c r="K36" s="36"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="58"/>
       <c r="B37" s="61"/>
       <c r="C37" s="62"/>
@@ -5332,16 +6631,16 @@
       <c r="J37" s="60"/>
       <c r="K37" s="57"/>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="50"/>
       <c r="B38" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="74">
         <f>J36</f>
         <v>426364.94493201922</v>
       </c>
-      <c r="D38" s="66"/>
+      <c r="D38" s="74"/>
       <c r="E38" s="39">
         <v>100</v>
       </c>
@@ -5352,15 +6651,15 @@
       <c r="J38" s="54"/>
       <c r="K38" s="55"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="56"/>
       <c r="B39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="69">
+      <c r="C39" s="77">
         <v>400000</v>
       </c>
-      <c r="D39" s="69"/>
+      <c r="D39" s="77"/>
       <c r="E39" s="39"/>
       <c r="F39" s="49"/>
       <c r="G39" s="48"/>
@@ -5369,16 +6668,16 @@
       <c r="J39" s="48"/>
       <c r="K39" s="49"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="56"/>
       <c r="B40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="69">
+      <c r="C40" s="77">
         <f>C39-C42-C43</f>
         <v>380000</v>
       </c>
-      <c r="D40" s="69"/>
+      <c r="D40" s="77"/>
       <c r="E40" s="39">
         <f>C40/C38*100</f>
         <v>89.125526035117218</v>
@@ -5390,16 +6689,16 @@
       <c r="J40" s="48"/>
       <c r="K40" s="49"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="56"/>
       <c r="B41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="66">
+      <c r="C41" s="74">
         <f>C38-C40</f>
         <v>46364.944932019222</v>
       </c>
-      <c r="D41" s="66"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="39">
         <f>100-E40</f>
         <v>10.874473964882782</v>
@@ -5411,16 +6710,16 @@
       <c r="J41" s="48"/>
       <c r="K41" s="49"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="56"/>
       <c r="B42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="66">
+      <c r="C42" s="74">
         <f>C39*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D42" s="66"/>
+      <c r="D42" s="74"/>
       <c r="E42" s="39">
         <v>3</v>
       </c>
@@ -5431,16 +6730,16 @@
       <c r="J42" s="48"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="56"/>
       <c r="B43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="66">
+      <c r="C43" s="74">
         <f>C39*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D43" s="66"/>
+      <c r="D43" s="74"/>
       <c r="E43" s="39">
         <v>2</v>
       </c>
@@ -5451,7 +6750,7 @@
       <c r="J43" s="48"/>
       <c r="K43" s="49"/>
     </row>
-    <row r="44" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="57"/>
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
@@ -5464,64 +6763,71 @@
       <c r="J44" s="57"/>
       <c r="K44" s="57"/>
     </row>
-    <row r="45" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="A7:F7"/>
@@ -5531,13 +6837,6 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="K15:K16"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>